<commit_message>
Updated Bug Logging Template and Testing Types Document
</commit_message>
<xml_diff>
--- a/OrangeHRM/OrangeHRM TestCases.xlsx
+++ b/OrangeHRM/OrangeHRM TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948724D5-BE73-48BE-8836-C9172ABD8F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B663AF-F80D-4D67-A6D0-7A3AC8515D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="153">
   <si>
     <t>SNO</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>TC_MyInfo_016</t>
-  </si>
-  <si>
-    <t>Orange HRM-MyInfo</t>
   </si>
   <si>
     <t>Verify login with valid ESS username and valid password.</t>
@@ -498,14 +495,84 @@
     <t>Verify ESS user able to delete  Dependants</t>
   </si>
   <si>
-    <t>Harsh@123/abcd</t>
+    <t>Username : Admin
+Password : admin123</t>
+  </si>
+  <si>
+    <t>Username : Admin
+Password : admin124</t>
+  </si>
+  <si>
+    <t>Username : Admin
+Password : admin125</t>
+  </si>
+  <si>
+    <t>Username : Admin
+Password : admin126</t>
+  </si>
+  <si>
+    <t>TC ID</t>
+  </si>
+  <si>
+    <t>Req ID</t>
+  </si>
+  <si>
+    <t>Orange HRM</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>TC_16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,6 +597,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -995,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1023,7 +1096,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
@@ -1121,7 +1194,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="15">
         <v>1</v>
@@ -1425,7 +1498,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="13"/>
     </row>
@@ -1535,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8314C97F-BF27-4FA3-8A3F-81D675E1385B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1556,13 +1629,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1574,7 +1647,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1588,10 +1661,10 @@
     </row>
     <row r="2" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>10</v>
@@ -1600,26 +1673,26 @@
         <v>11</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>10</v>
@@ -1628,26 +1701,26 @@
         <v>11</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>131</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>10</v>
@@ -1656,26 +1729,26 @@
         <v>11</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>10</v>
@@ -1684,54 +1757,54 @@
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>10</v>
@@ -1740,26 +1813,26 @@
         <v>16</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>10</v>
@@ -1768,26 +1841,26 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>13</v>
@@ -1796,13 +1869,13 @@
         <v>14</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -1810,10 +1883,10 @@
     </row>
     <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>15</v>
@@ -1822,26 +1895,26 @@
         <v>19</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>15</v>
@@ -1850,26 +1923,26 @@
         <v>20</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>17</v>
@@ -1878,26 +1951,26 @@
         <v>21</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>17</v>
@@ -1906,26 +1979,26 @@
         <v>22</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>17</v>
@@ -1934,26 +2007,26 @@
         <v>23</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" ht="156" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>18</v>
@@ -1962,26 +2035,26 @@
         <v>24</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>18</v>
@@ -1990,26 +2063,26 @@
         <v>25</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>18</v>
@@ -2018,26 +2091,27 @@
         <v>26</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{A6B33591-4D10-45DA-A04C-F5FF0D6B85F8}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{2D1E6DD5-8B87-40BB-9501-8BB0FFBFE584}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{4B68E6C7-21AC-41AB-A3D9-64D416FC23E9}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{6394B160-4731-4351-B511-74AA95348B93}"/>
+    <hyperlink ref="G2" r:id="rId1" display="Harsh@123/abcd" xr:uid="{A6B33591-4D10-45DA-A04C-F5FF0D6B85F8}"/>
+    <hyperlink ref="G3" r:id="rId2" display="Harsh@123/abcd" xr:uid="{1FC074B1-2586-49BC-A05B-1590A4589E3D}"/>
+    <hyperlink ref="G4" r:id="rId3" display="Harsh@123/abcd" xr:uid="{04B94B17-A817-4623-ADA8-92D4A9822879}"/>
+    <hyperlink ref="G5" r:id="rId4" display="Harsh@123/abcd" xr:uid="{1E969E14-E946-4160-B5A9-4610FD3D93EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>

</xml_diff>